<commit_message>
add feature and upload data from excel
</commit_message>
<xml_diff>
--- a/src/test/resources/dataEntry.xlsx
+++ b/src/test/resources/dataEntry.xlsx
@@ -5,19 +5,20 @@
   <sheets>
     <sheet state="visible" name="test1" sheetId="1" r:id="rId4"/>
     <sheet state="visible" name="test2" sheetId="2" r:id="rId5"/>
+    <sheet state="visible" name="transferTest1" sheetId="3" r:id="rId6"/>
   </sheets>
   <definedNames/>
   <calcPr/>
   <extLst>
     <ext uri="GoogleSheetsCustomDataVersion2">
-      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId6" roundtripDataChecksum="gNQqN9/D0A32qpTanNMc1D8Sti6O9TtAAcOdyyiKFlU="/>
+      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId7" roundtripDataChecksum="3spYtSaBRmW2Dbh276gP6sol2C99vaW4piiM7dpBA/A="/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="20">
   <si>
     <t>username</t>
   </si>
@@ -47,12 +48,45 @@
   </si>
   <si>
     <t>usetest2@yopmail.com</t>
+  </si>
+  <si>
+    <t>bankName</t>
+  </si>
+  <si>
+    <t>dateTransfer</t>
+  </si>
+  <si>
+    <t>userTansfer1</t>
+  </si>
+  <si>
+    <t>PaSSword123*-/&amp;</t>
+  </si>
+  <si>
+    <t>usertransfer@yopmail.com</t>
+  </si>
+  <si>
+    <t>Banco Tierra</t>
+  </si>
+  <si>
+    <t>userTansfer2</t>
+  </si>
+  <si>
+    <t>PaSS/*-35,%#word</t>
+  </si>
+  <si>
+    <t>usertransfer2@yopmail.com</t>
+  </si>
+  <si>
+    <t>Banco ABC</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="dd/mm/yyyy"/>
+  </numFmts>
   <fonts count="2">
     <font>
       <sz val="11.0"/>
@@ -80,11 +114,14 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment readingOrder="0"/>
     </xf>
   </cellXfs>
@@ -100,6 +137,10 @@
 </file>
 
 <file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
 </file>
 
@@ -1384,4 +1425,83 @@
   </sheetData>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="0" summaryRight="0"/>
+  </sheetPr>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.0"/>
+  <cols>
+    <col customWidth="1" min="2" max="2" width="17.14"/>
+    <col customWidth="1" min="3" max="3" width="24.29"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D2" s="1">
+        <v>89.54</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2" s="2">
+        <v>45424.0</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D3" s="1">
+        <v>15.08</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F3" s="2">
+        <v>40462.0</v>
+      </c>
+    </row>
+  </sheetData>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>